<commit_message>
add hours week 3
</commit_message>
<xml_diff>
--- a/time_sheet/KidSports_CS297-TimeTracking.xlsx
+++ b/time_sheet/KidSports_CS297-TimeTracking.xlsx
@@ -182,7 +182,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,11 +308,11 @@
         <v>45</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">D6+E5</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">F6+G5</f>
@@ -333,7 +333,7 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7+E6</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">F7+G6</f>
@@ -354,7 +354,7 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">F8+G7</f>
@@ -375,7 +375,7 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">F9+G8</f>
@@ -396,7 +396,7 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">F10+G9</f>
@@ -417,7 +417,7 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">F11+G10</f>
@@ -438,7 +438,7 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">F12+G11</f>
@@ -459,7 +459,7 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">F13+G12</f>

</xml_diff>

<commit_message>
add button name and value attribute, add hours
</commit_message>
<xml_diff>
--- a/time_sheet/KidSports_CS297-TimeTracking.xlsx
+++ b/time_sheet/KidSports_CS297-TimeTracking.xlsx
@@ -176,14 +176,11 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5674418604651"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -327,13 +324,19 @@
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="C7" s="0" t="n">
         <f aca="false">B7+C6</f>
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7+E6</f>
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">F7+G6</f>
@@ -348,13 +351,19 @@
       <c r="A8" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="0" t="n">
+        <v>18</v>
+      </c>
       <c r="C8" s="0" t="n">
         <f aca="false">B8+C7</f>
-        <v>45</v>
+        <v>75</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">F8+G7</f>
@@ -369,13 +378,19 @@
       <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9+C8</f>
-        <v>45</v>
+        <v>90</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">F9+G8</f>
@@ -392,11 +407,11 @@
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10+C9</f>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">F10+G9</f>
@@ -413,11 +428,11 @@
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">B11+C10</f>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">F11+G10</f>
@@ -434,11 +449,11 @@
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">B12+C11</f>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">F12+G11</f>
@@ -455,11 +470,11 @@
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">B13+C12</f>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">F13+G12</f>

</xml_diff>